<commit_message>
APACHE POI Reading from Excel
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekchicago-1/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekchicago-1/Desktop/cybertek21-cucumber-junit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D88F4D2-2BEB-6140-A265-25E1E013CAAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC81486-2CA0-5A4B-8485-48FFB600D7FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="2580" windowWidth="28040" windowHeight="17440" xr2:uid="{973C79E2-212B-7C44-A95E-272F10C99F5C}"/>
+    <workbookView xWindow="6760" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{973C79E2-212B-7C44-A95E-272F10C99F5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
APACHE POI Writing to Excel
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekchicago-1/Desktop/cybertek21-cucumber-junit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDA5CF5-046F-7D42-BF0D-30CE0157B487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABA3ECC-1791-1B41-ACF9-E84271D14269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6760" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{973C79E2-212B-7C44-A95E-272F10C99F5C}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>FirstName</t>
   </si>
@@ -76,12 +76,16 @@
   </si>
   <si>
     <t>SDET</t>
+  </si>
+  <si>
+    <t>Madam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -430,7 +434,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,7 +463,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
APACHE POI  SELENIUM IMPLEMENTATION
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekchicago-1/Desktop/cybertek21-cucumber-junit/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>FirstName</t>
   </si>
@@ -76,12 +76,19 @@
   </si>
   <si>
     <t>SDET</t>
+  </si>
+  <si>
+    <t>Madam</t>
+  </si>
+  <si>
+    <t>Tom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -448,7 +455,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -459,7 +466,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>

</xml_diff>